<commit_message>
Actualización guion y escaleta CN 06 04
Actualización guion y escaleta CN 06 04
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Dropbox\Editorial planeta\1. Autor\Escaletas\CN_06_04_CO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Escaleta" sheetId="2" r:id="rId1"/>
     <sheet name="VER" sheetId="3" r:id="rId2"/>
-    <sheet name="DATOS" sheetId="1" r:id="rId3"/>
+    <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Escaleta!$A$2:$U$38</definedName>
@@ -391,9 +396,6 @@
     <t>CN_06_04_CO</t>
   </si>
   <si>
-    <t>La nutrición</t>
-  </si>
-  <si>
     <t>RM</t>
   </si>
   <si>
@@ -830,6 +832,9 @@
   </si>
   <si>
     <t>La nutrición de los seres vivos</t>
+  </si>
+  <si>
+    <t>La nutrición en los seres vivos</t>
   </si>
 </sst>
 </file>
@@ -1219,34 +1224,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1286,6 +1273,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1349,7 +1354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1384,7 +1389,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1593,11 +1598,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:U123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K35" sqref="A35:XFD35"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,8 +1620,8 @@
     <col min="11" max="11" width="13.28515625" customWidth="1"/>
     <col min="12" max="12" width="25.7109375" customWidth="1"/>
     <col min="13" max="14" width="9.28515625" customWidth="1"/>
-    <col min="15" max="15" width="3.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="1" customWidth="1"/>
     <col min="17" max="17" width="20.42578125" style="1" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -1624,94 +1630,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="75" t="s">
+      <c r="H1" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="75" t="s">
+      <c r="I1" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="J1" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="83" t="s">
+      <c r="K1" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="81" t="s">
+      <c r="L1" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="87" t="s">
+      <c r="M1" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="87"/>
-      <c r="O1" s="67" t="s">
+      <c r="N1" s="81"/>
+      <c r="O1" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="69" t="s">
+      <c r="Q1" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="73" t="s">
+      <c r="R1" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="69" t="s">
+      <c r="S1" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="71" t="s">
+      <c r="T1" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="69" t="s">
+      <c r="U1" s="84" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="80"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="82"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="76"/>
       <c r="M2" s="14" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="89"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="85"/>
     </row>
     <row r="3" spans="1:21" s="47" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -1721,17 +1727,17 @@
         <v>122</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D3" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="61" t="s">
         <v>224</v>
-      </c>
-      <c r="E3" s="61" t="s">
-        <v>225</v>
       </c>
       <c r="F3" s="37"/>
       <c r="G3" s="32" t="s">
-        <v>123</v>
+        <v>269</v>
       </c>
       <c r="H3" s="38">
         <v>1</v>
@@ -1740,7 +1746,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K3" s="41" t="s">
         <v>20</v>
@@ -1760,16 +1766,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="S3" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="S3" s="45" t="s">
+      <c r="T3" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="T3" s="64" t="s">
+      <c r="U3" s="45" t="s">
         <v>126</v>
-      </c>
-      <c r="U3" s="45" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1780,17 +1786,17 @@
         <v>122</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D4" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" s="62" t="s">
         <v>224</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>225</v>
       </c>
       <c r="F4" s="52"/>
       <c r="G4" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H4" s="53">
         <v>2</v>
@@ -1799,7 +1805,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="55" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K4" s="56" t="s">
         <v>20</v>
@@ -1819,19 +1825,19 @@
         <v>6</v>
       </c>
       <c r="R4" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S4" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T4" s="65" t="s">
+        <v>239</v>
+      </c>
+      <c r="U4" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="T4" s="65" t="s">
-        <v>240</v>
-      </c>
-      <c r="U4" s="59" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:21" s="47" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>17</v>
       </c>
@@ -1839,16 +1845,16 @@
         <v>122</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G5" s="31"/>
       <c r="H5" s="53"/>
@@ -1874,19 +1880,19 @@
         <v>122</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H6" s="53">
         <v>3</v>
@@ -1895,7 +1901,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="55" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K6" s="56" t="s">
         <v>20</v>
@@ -1915,16 +1921,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="S6" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="S6" s="59" t="s">
+      <c r="T6" s="65" t="s">
+        <v>236</v>
+      </c>
+      <c r="U6" s="59" t="s">
         <v>141</v>
-      </c>
-      <c r="T6" s="65" t="s">
-        <v>237</v>
-      </c>
-      <c r="U6" s="59" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1935,19 +1941,19 @@
         <v>122</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H7" s="53">
         <v>4</v>
@@ -1956,7 +1962,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K7" s="56" t="s">
         <v>20</v>
@@ -1976,16 +1982,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S7" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T7" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="U7" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T7" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="U7" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -1996,19 +2002,19 @@
         <v>122</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H8" s="53">
         <v>5</v>
@@ -2017,7 +2023,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="55" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K8" s="56" t="s">
         <v>20</v>
@@ -2037,16 +2043,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S8" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T8" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="U8" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T8" s="65" t="s">
-        <v>241</v>
-      </c>
-      <c r="U8" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2057,19 +2063,19 @@
         <v>122</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H9" s="53">
         <v>6</v>
@@ -2078,7 +2084,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K9" s="56" t="s">
         <v>20</v>
@@ -2098,16 +2104,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S9" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T9" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="U9" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T9" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="U9" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2118,17 +2124,17 @@
         <v>122</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E10" s="62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F10" s="52"/>
       <c r="G10" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H10" s="53">
         <v>7</v>
@@ -2137,7 +2143,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="55" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K10" s="56" t="s">
         <v>20</v>
@@ -2157,16 +2163,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S10" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T10" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="U10" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T10" s="65" t="s">
-        <v>137</v>
-      </c>
-      <c r="U10" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2177,17 +2183,17 @@
         <v>122</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H11" s="53">
         <v>8</v>
@@ -2196,7 +2202,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="55" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K11" s="56" t="s">
         <v>20</v>
@@ -2205,7 +2211,7 @@
         <v>5</v>
       </c>
       <c r="M11" s="58" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N11" s="58"/>
       <c r="O11" s="52"/>
@@ -2216,16 +2222,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="S11" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="S11" s="59" t="s">
+      <c r="T11" s="65" t="s">
+        <v>244</v>
+      </c>
+      <c r="U11" s="59" t="s">
         <v>141</v>
-      </c>
-      <c r="T11" s="65" t="s">
-        <v>245</v>
-      </c>
-      <c r="U11" s="59" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2236,19 +2242,19 @@
         <v>122</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E12" s="62" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H12" s="53">
         <v>9</v>
@@ -2257,7 +2263,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K12" s="56" t="s">
         <v>20</v>
@@ -2277,19 +2283,19 @@
         <v>6</v>
       </c>
       <c r="R12" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S12" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T12" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="U12" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="T12" s="65" t="s">
-        <v>163</v>
-      </c>
-      <c r="U12" s="59" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
         <v>17</v>
       </c>
@@ -2297,16 +2303,16 @@
         <v>122</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E13" s="62" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G13" s="31"/>
       <c r="H13" s="53"/>
@@ -2332,19 +2338,19 @@
         <v>122</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E14" s="62" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F14" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="31" t="s">
         <v>146</v>
-      </c>
-      <c r="G14" s="31" t="s">
-        <v>147</v>
       </c>
       <c r="H14" s="53">
         <v>10</v>
@@ -2353,7 +2359,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K14" s="56" t="s">
         <v>20</v>
@@ -2373,16 +2379,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S14" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T14" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="U14" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T14" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="U14" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2393,19 +2399,19 @@
         <v>122</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E15" s="62" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H15" s="53">
         <v>11</v>
@@ -2414,7 +2420,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K15" s="56" t="s">
         <v>20</v>
@@ -2434,16 +2440,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S15" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T15" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="U15" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T15" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="U15" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -2454,17 +2460,17 @@
         <v>122</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F16" s="52"/>
       <c r="G16" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H16" s="53">
         <v>12</v>
@@ -2473,7 +2479,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="55" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K16" s="56" t="s">
         <v>20</v>
@@ -2493,16 +2499,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S16" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T16" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="U16" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T16" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="U16" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2513,15 +2519,15 @@
         <v>122</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E17" s="62"/>
       <c r="F17" s="52"/>
       <c r="G17" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H17" s="53">
         <v>13</v>
@@ -2530,7 +2536,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K17" s="56" t="s">
         <v>20</v>
@@ -2550,16 +2556,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="S17" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="S17" s="59" t="s">
+      <c r="T17" s="65" t="s">
+        <v>251</v>
+      </c>
+      <c r="U17" s="59" t="s">
         <v>141</v>
-      </c>
-      <c r="T17" s="65" t="s">
-        <v>252</v>
-      </c>
-      <c r="U17" s="59" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2570,15 +2576,15 @@
         <v>122</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E18" s="62"/>
       <c r="F18" s="52"/>
       <c r="G18" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H18" s="53">
         <v>14</v>
@@ -2587,7 +2593,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K18" s="56" t="s">
         <v>20</v>
@@ -2607,16 +2613,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S18" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T18" s="65" t="s">
+        <v>155</v>
+      </c>
+      <c r="U18" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T18" s="65" t="s">
-        <v>156</v>
-      </c>
-      <c r="U18" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2627,15 +2633,15 @@
         <v>122</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E19" s="62"/>
       <c r="F19" s="52"/>
       <c r="G19" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H19" s="53">
         <v>15</v>
@@ -2644,7 +2650,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="55" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K19" s="56" t="s">
         <v>20</v>
@@ -2664,16 +2670,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S19" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T19" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="U19" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T19" s="65" t="s">
-        <v>159</v>
-      </c>
-      <c r="U19" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2684,17 +2690,17 @@
         <v>122</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F20" s="52"/>
       <c r="G20" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H20" s="53">
         <v>16</v>
@@ -2703,7 +2709,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K20" s="56" t="s">
         <v>20</v>
@@ -2723,16 +2729,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S20" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T20" s="65" t="s">
+        <v>247</v>
+      </c>
+      <c r="U20" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T20" s="65" t="s">
-        <v>248</v>
-      </c>
-      <c r="U20" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -2743,17 +2749,17 @@
         <v>122</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E21" s="62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F21" s="52"/>
       <c r="G21" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H21" s="53">
         <v>17</v>
@@ -2762,7 +2768,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K21" s="56" t="s">
         <v>20</v>
@@ -2782,19 +2788,19 @@
         <v>6</v>
       </c>
       <c r="R21" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S21" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T21" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="U21" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="T21" s="65" t="s">
-        <v>144</v>
-      </c>
-      <c r="U21" s="59" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:21" s="47" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>17</v>
       </c>
@@ -2802,13 +2808,13 @@
         <v>122</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E22" s="62" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F22" s="52"/>
       <c r="G22" s="31"/>
@@ -2835,17 +2841,17 @@
         <v>122</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E23" s="62" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F23" s="52"/>
       <c r="G23" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H23" s="53">
         <v>18</v>
@@ -2854,7 +2860,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K23" s="56" t="s">
         <v>20</v>
@@ -2874,16 +2880,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S23" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T23" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="U23" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T23" s="65" t="s">
-        <v>168</v>
-      </c>
-      <c r="U23" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2894,17 +2900,17 @@
         <v>122</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F24" s="52"/>
       <c r="G24" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H24" s="53">
         <v>19</v>
@@ -2913,7 +2919,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="55" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K24" s="56" t="s">
         <v>20</v>
@@ -2933,19 +2939,19 @@
         <v>6</v>
       </c>
       <c r="R24" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S24" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T24" s="65" t="s">
+        <v>168</v>
+      </c>
+      <c r="U24" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="T24" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="U24" s="59" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>17</v>
       </c>
@@ -2953,17 +2959,17 @@
         <v>122</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E25" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F25" s="52"/>
       <c r="G25" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H25" s="53">
         <v>20</v>
@@ -2972,7 +2978,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="55" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K25" s="56" t="s">
         <v>19</v>
@@ -2989,22 +2995,22 @@
         <v>19</v>
       </c>
       <c r="Q25" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="R25" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="R25" s="60" t="s">
+      <c r="S25" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="S25" s="59" t="s">
+      <c r="T25" s="65" t="s">
+        <v>257</v>
+      </c>
+      <c r="U25" s="59" t="s">
         <v>177</v>
       </c>
-      <c r="T25" s="65" t="s">
-        <v>258</v>
-      </c>
-      <c r="U25" s="59" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>17</v>
       </c>
@@ -3012,17 +3018,17 @@
         <v>122</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D26" s="51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E26" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F26" s="52"/>
       <c r="G26" s="31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H26" s="53">
         <v>21</v>
@@ -3031,7 +3037,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K26" s="56" t="s">
         <v>19</v>
@@ -3048,19 +3054,19 @@
         <v>19</v>
       </c>
       <c r="Q26" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="R26" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="R26" s="60" t="s">
+      <c r="S26" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="S26" s="59" t="s">
+      <c r="T26" s="65" t="s">
+        <v>172</v>
+      </c>
+      <c r="U26" s="59" t="s">
         <v>177</v>
-      </c>
-      <c r="T26" s="65" t="s">
-        <v>173</v>
-      </c>
-      <c r="U26" s="59" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3071,17 +3077,17 @@
         <v>122</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D27" s="51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E27" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F27" s="52"/>
       <c r="G27" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H27" s="53">
         <v>22</v>
@@ -3090,7 +3096,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K27" s="56" t="s">
         <v>20</v>
@@ -3110,16 +3116,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S27" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T27" s="65" t="s">
+        <v>259</v>
+      </c>
+      <c r="U27" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T27" s="65" t="s">
-        <v>260</v>
-      </c>
-      <c r="U27" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3130,17 +3136,17 @@
         <v>122</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D28" s="51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E28" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F28" s="52"/>
       <c r="G28" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H28" s="53">
         <v>23</v>
@@ -3149,7 +3155,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="55" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K28" s="56" t="s">
         <v>20</v>
@@ -3169,19 +3175,19 @@
         <v>6</v>
       </c>
       <c r="R28" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="S28" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="S28" s="59" t="s">
+      <c r="T28" s="65" t="s">
+        <v>267</v>
+      </c>
+      <c r="U28" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="T28" s="65" t="s">
-        <v>268</v>
-      </c>
-      <c r="U28" s="59" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
         <v>17</v>
       </c>
@@ -3189,17 +3195,17 @@
         <v>122</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D29" s="51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F29" s="52"/>
       <c r="G29" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H29" s="53">
         <v>24</v>
@@ -3208,7 +3214,7 @@
         <v>19</v>
       </c>
       <c r="J29" s="55" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K29" s="56" t="s">
         <v>19</v>
@@ -3225,22 +3231,22 @@
         <v>19</v>
       </c>
       <c r="Q29" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="R29" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="R29" s="60" t="s">
-        <v>176</v>
-      </c>
       <c r="S29" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="T29" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="U29" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="T29" s="65" t="s">
-        <v>182</v>
-      </c>
-      <c r="U29" s="59" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
         <v>17</v>
       </c>
@@ -3248,17 +3254,17 @@
         <v>122</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D30" s="51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E30" s="62" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F30" s="52"/>
       <c r="G30" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H30" s="53">
         <v>25</v>
@@ -3267,7 +3273,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="55" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K30" s="56" t="s">
         <v>19</v>
@@ -3284,19 +3290,19 @@
         <v>19</v>
       </c>
       <c r="Q30" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="R30" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="R30" s="60" t="s">
-        <v>176</v>
-      </c>
       <c r="S30" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="T30" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="U30" s="59" t="s">
         <v>184</v>
-      </c>
-      <c r="T30" s="65" t="s">
-        <v>186</v>
-      </c>
-      <c r="U30" s="59" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3307,17 +3313,17 @@
         <v>122</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E31" s="62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F31" s="52"/>
       <c r="G31" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H31" s="53">
         <v>26</v>
@@ -3326,7 +3332,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K31" s="56" t="s">
         <v>20</v>
@@ -3346,19 +3352,19 @@
         <v>6</v>
       </c>
       <c r="R31" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S31" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T31" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="U31" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="T31" s="65" t="s">
-        <v>189</v>
-      </c>
-      <c r="U31" s="59" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
         <v>17</v>
       </c>
@@ -3366,15 +3372,15 @@
         <v>122</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D32" s="51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E32" s="62"/>
       <c r="F32" s="52"/>
       <c r="G32" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H32" s="53">
         <v>27</v>
@@ -3383,7 +3389,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="55" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K32" s="56" t="s">
         <v>19</v>
@@ -3393,29 +3399,29 @@
       </c>
       <c r="M32" s="58"/>
       <c r="N32" s="58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O32" s="52"/>
       <c r="P32" s="52" t="s">
         <v>19</v>
       </c>
       <c r="Q32" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="R32" s="60" t="s">
+        <v>175</v>
+      </c>
+      <c r="S32" s="59" t="s">
         <v>194</v>
       </c>
-      <c r="R32" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="S32" s="59" t="s">
+      <c r="T32" s="65" t="s">
+        <v>190</v>
+      </c>
+      <c r="U32" s="59" t="s">
         <v>195</v>
       </c>
-      <c r="T32" s="65" t="s">
-        <v>191</v>
-      </c>
-      <c r="U32" s="59" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
         <v>17</v>
       </c>
@@ -3423,15 +3429,15 @@
         <v>122</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E33" s="62"/>
       <c r="F33" s="52"/>
       <c r="G33" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H33" s="53">
         <v>28</v>
@@ -3440,7 +3446,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K33" s="56" t="s">
         <v>19</v>
@@ -3450,29 +3456,29 @@
       </c>
       <c r="M33" s="58"/>
       <c r="N33" s="58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O33" s="52"/>
       <c r="P33" s="52" t="s">
         <v>19</v>
       </c>
       <c r="Q33" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="R33" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="R33" s="60" t="s">
+      <c r="S33" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="S33" s="59" t="s">
+      <c r="T33" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="U33" s="59" t="s">
         <v>177</v>
       </c>
-      <c r="T33" s="65" t="s">
-        <v>197</v>
-      </c>
-      <c r="U33" s="59" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
         <v>17</v>
       </c>
@@ -3480,15 +3486,15 @@
         <v>122</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D34" s="51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E34" s="62"/>
       <c r="F34" s="52"/>
       <c r="G34" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H34" s="53">
         <v>29</v>
@@ -3497,7 +3503,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K34" s="56" t="s">
         <v>19</v>
@@ -3507,43 +3513,43 @@
       </c>
       <c r="M34" s="58"/>
       <c r="N34" s="58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O34" s="52"/>
       <c r="P34" s="52" t="s">
         <v>19</v>
       </c>
       <c r="Q34" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="R34" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="R34" s="60" t="s">
-        <v>176</v>
-      </c>
       <c r="S34" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="T34" s="65" t="s">
+        <v>198</v>
+      </c>
+      <c r="U34" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="T34" s="65" t="s">
-        <v>199</v>
-      </c>
-      <c r="U34" s="59" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" s="47" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:21" s="47" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48"/>
       <c r="B35" s="49" t="s">
         <v>122</v>
       </c>
       <c r="C35" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D35" s="51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E35" s="62"/>
       <c r="F35" s="52"/>
       <c r="G35" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H35" s="53">
         <v>30</v>
@@ -3552,7 +3558,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K35" s="56" t="s">
         <v>19</v>
@@ -3562,26 +3568,26 @@
       </c>
       <c r="M35" s="58"/>
       <c r="N35" s="58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O35" s="52"/>
       <c r="P35" s="52" t="s">
         <v>19</v>
       </c>
       <c r="Q35" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="R35" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="R35" s="60" t="s">
-        <v>176</v>
-      </c>
       <c r="S35" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="T35" s="65" t="s">
+        <v>263</v>
+      </c>
+      <c r="U35" s="59" t="s">
         <v>184</v>
-      </c>
-      <c r="T35" s="65" t="s">
-        <v>264</v>
-      </c>
-      <c r="U35" s="59" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -3592,15 +3598,15 @@
         <v>122</v>
       </c>
       <c r="C36" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D36" s="51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E36" s="62"/>
       <c r="F36" s="52"/>
       <c r="G36" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H36" s="53">
         <v>31</v>
@@ -3609,7 +3615,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K36" s="56" t="s">
         <v>20</v>
@@ -3637,15 +3643,15 @@
         <v>122</v>
       </c>
       <c r="C37" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D37" s="51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E37" s="62"/>
       <c r="F37" s="52"/>
       <c r="G37" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H37" s="53">
         <v>32</v>
@@ -3654,7 +3660,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="55" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K37" s="56" t="s">
         <v>20</v>
@@ -3674,16 +3680,16 @@
         <v>6</v>
       </c>
       <c r="R37" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S37" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T37" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="U37" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T37" s="65" t="s">
-        <v>206</v>
-      </c>
-      <c r="U37" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -3694,24 +3700,24 @@
         <v>122</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D38" s="51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E38" s="62"/>
       <c r="F38" s="52"/>
       <c r="G38" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H38" s="53">
         <v>33</v>
       </c>
       <c r="I38" s="54" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J38" s="55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K38" s="56" t="s">
         <v>20</v>
@@ -3731,16 +3737,16 @@
         <v>6</v>
       </c>
       <c r="R38" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S38" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T38" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="U38" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="T38" s="65" t="s">
-        <v>209</v>
-      </c>
-      <c r="U38" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4711,7 +4717,20 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:U38">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="NO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4726,12 +4745,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4793,114 +4806,114 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="21" t="s">
         <v>213</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="24"/>
       <c r="D3" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="D8" s="28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="D9" s="28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E9" s="29"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
       <c r="D10" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E10" s="29"/>
     </row>

</xml_diff>

<commit_message>
Actualización Docs CN 06 04
Actualización Docs CN 06 04
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Dropbox\Editorial planeta\1. Autor\Escaletas\CN_06_04_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1224,16 +1224,34 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1273,24 +1291,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1598,12 +1598,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:U123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,94 +1629,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="75" t="s">
+      <c r="G1" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="J1" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="77" t="s">
+      <c r="K1" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="75" t="s">
+      <c r="L1" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="81" t="s">
+      <c r="M1" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="81"/>
-      <c r="O1" s="69" t="s">
+      <c r="N1" s="87"/>
+      <c r="O1" s="67" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="69" t="s">
+      <c r="P1" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="84" t="s">
+      <c r="Q1" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="88" t="s">
+      <c r="R1" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="84" t="s">
+      <c r="S1" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="86" t="s">
+      <c r="T1" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="84" t="s">
+      <c r="U1" s="69" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="76"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="82"/>
       <c r="M2" s="14" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="85"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="70"/>
     </row>
     <row r="3" spans="1:21" s="47" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -1837,7 +1836,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="47" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>17</v>
       </c>
@@ -2295,7 +2294,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
         <v>17</v>
       </c>
@@ -2800,7 +2799,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="47" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>17</v>
       </c>
@@ -2951,7 +2950,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>17</v>
       </c>
@@ -3010,7 +3009,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>17</v>
       </c>
@@ -3187,7 +3186,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
         <v>17</v>
       </c>
@@ -3246,7 +3245,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
         <v>17</v>
       </c>
@@ -3364,7 +3363,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
         <v>17</v>
       </c>
@@ -3421,7 +3420,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
         <v>17</v>
       </c>
@@ -3478,7 +3477,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
         <v>17</v>
       </c>
@@ -3535,7 +3534,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="47" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" s="47" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48"/>
       <c r="B35" s="49" t="s">
         <v>122</v>
@@ -4717,20 +4716,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U38">
-    <filterColumn colId="10">
-      <filters>
-        <filter val="NO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:U38"/>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4745,6 +4732,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización CN 06 04
Actualización CN 06 04
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
@@ -1224,34 +1224,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1291,6 +1273,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1600,9 +1600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,94 +1629,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="75" t="s">
+      <c r="H1" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="75" t="s">
+      <c r="I1" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="J1" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="83" t="s">
+      <c r="K1" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="81" t="s">
+      <c r="L1" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="87" t="s">
+      <c r="M1" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="87"/>
-      <c r="O1" s="67" t="s">
+      <c r="N1" s="81"/>
+      <c r="O1" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="69" t="s">
+      <c r="Q1" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="73" t="s">
+      <c r="R1" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="69" t="s">
+      <c r="S1" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="71" t="s">
+      <c r="T1" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="69" t="s">
+      <c r="U1" s="84" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="80"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="82"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="76"/>
       <c r="M2" s="14" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="89"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="85"/>
     </row>
     <row r="3" spans="1:21" s="47" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -4718,6 +4718,12 @@
   </sheetData>
   <autoFilter ref="A2:U38"/>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4732,12 +4738,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización escaleta CN 06 04
Actualización escaleta CN 06 04
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Dropbox\Editorial planeta\1. Autor\Escaletas\CN_06_04_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="271">
   <si>
     <t>Asignatura</t>
   </si>
@@ -747,9 +747,6 @@
     <t>Recurso M5A-01</t>
   </si>
   <si>
-    <t>Recurso M9B-01</t>
-  </si>
-  <si>
     <t>Actividad acerca del concepto de la nutrición</t>
   </si>
   <si>
@@ -835,6 +832,12 @@
   </si>
   <si>
     <t>La nutrición en los seres vivos</t>
+  </si>
+  <si>
+    <t>m12A</t>
+  </si>
+  <si>
+    <t>Recurso M12A-01</t>
   </si>
 </sst>
 </file>
@@ -1224,16 +1227,34 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1273,24 +1294,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1598,11 +1601,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:U123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,94 +1633,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="75" t="s">
+      <c r="G1" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="J1" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="77" t="s">
+      <c r="K1" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="75" t="s">
+      <c r="L1" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="81" t="s">
+      <c r="M1" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="81"/>
-      <c r="O1" s="69" t="s">
+      <c r="N1" s="87"/>
+      <c r="O1" s="67" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="69" t="s">
+      <c r="P1" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="84" t="s">
+      <c r="Q1" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="88" t="s">
+      <c r="R1" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="84" t="s">
+      <c r="S1" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="86" t="s">
+      <c r="T1" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="84" t="s">
+      <c r="U1" s="69" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="76"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="82"/>
       <c r="M2" s="14" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="85"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="70"/>
     </row>
     <row r="3" spans="1:21" s="47" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -1726,7 +1730,7 @@
         <v>122</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>223</v>
@@ -1736,7 +1740,7 @@
       </c>
       <c r="F3" s="37"/>
       <c r="G3" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H3" s="38">
         <v>1</v>
@@ -1785,7 +1789,7 @@
         <v>122</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" s="51" t="s">
         <v>223</v>
@@ -1836,7 +1840,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="47" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>17</v>
       </c>
@@ -1844,7 +1848,7 @@
         <v>122</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D5" s="51" t="s">
         <v>223</v>
@@ -1879,7 +1883,7 @@
         <v>122</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D6" s="51" t="s">
         <v>223</v>
@@ -1940,7 +1944,7 @@
         <v>122</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D7" s="51" t="s">
         <v>223</v>
@@ -2001,7 +2005,7 @@
         <v>122</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D8" s="51" t="s">
         <v>223</v>
@@ -2022,7 +2026,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="55" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K8" s="56" t="s">
         <v>20</v>
@@ -2032,7 +2036,7 @@
       </c>
       <c r="M8" s="58"/>
       <c r="N8" s="58" t="s">
-        <v>41</v>
+        <v>269</v>
       </c>
       <c r="O8" s="52"/>
       <c r="P8" s="52" t="s">
@@ -2048,7 +2052,7 @@
         <v>127</v>
       </c>
       <c r="T8" s="65" t="s">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="U8" s="59" t="s">
         <v>128</v>
@@ -2062,7 +2066,7 @@
         <v>122</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D9" s="51" t="s">
         <v>223</v>
@@ -2123,7 +2127,7 @@
         <v>122</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D10" s="51" t="s">
         <v>223</v>
@@ -2142,7 +2146,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="55" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K10" s="56" t="s">
         <v>20</v>
@@ -2182,7 +2186,7 @@
         <v>122</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D11" s="51" t="s">
         <v>137</v>
@@ -2201,7 +2205,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="55" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K11" s="56" t="s">
         <v>20</v>
@@ -2210,7 +2214,7 @@
         <v>5</v>
       </c>
       <c r="M11" s="58" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N11" s="58"/>
       <c r="O11" s="52"/>
@@ -2227,7 +2231,7 @@
         <v>140</v>
       </c>
       <c r="T11" s="65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U11" s="59" t="s">
         <v>141</v>
@@ -2241,7 +2245,7 @@
         <v>122</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D12" s="51" t="s">
         <v>137</v>
@@ -2262,7 +2266,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="55" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K12" s="56" t="s">
         <v>20</v>
@@ -2294,7 +2298,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
         <v>17</v>
       </c>
@@ -2302,7 +2306,7 @@
         <v>122</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D13" s="51" t="s">
         <v>137</v>
@@ -2337,7 +2341,7 @@
         <v>122</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D14" s="51" t="s">
         <v>137</v>
@@ -2398,7 +2402,7 @@
         <v>122</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D15" s="51" t="s">
         <v>137</v>
@@ -2419,7 +2423,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K15" s="56" t="s">
         <v>20</v>
@@ -2459,7 +2463,7 @@
         <v>122</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D16" s="51" t="s">
         <v>137</v>
@@ -2478,7 +2482,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="55" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K16" s="56" t="s">
         <v>20</v>
@@ -2518,7 +2522,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D17" s="51" t="s">
         <v>228</v>
@@ -2526,7 +2530,7 @@
       <c r="E17" s="62"/>
       <c r="F17" s="52"/>
       <c r="G17" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H17" s="53">
         <v>13</v>
@@ -2561,7 +2565,7 @@
         <v>140</v>
       </c>
       <c r="T17" s="65" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="U17" s="59" t="s">
         <v>141</v>
@@ -2575,7 +2579,7 @@
         <v>122</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D18" s="51" t="s">
         <v>228</v>
@@ -2583,7 +2587,7 @@
       <c r="E18" s="62"/>
       <c r="F18" s="52"/>
       <c r="G18" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H18" s="53">
         <v>14</v>
@@ -2632,7 +2636,7 @@
         <v>122</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D19" s="51" t="s">
         <v>228</v>
@@ -2689,7 +2693,7 @@
         <v>122</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D20" s="51" t="s">
         <v>228</v>
@@ -2734,7 +2738,7 @@
         <v>127</v>
       </c>
       <c r="T20" s="65" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="U20" s="59" t="s">
         <v>128</v>
@@ -2748,7 +2752,7 @@
         <v>122</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D21" s="51" t="s">
         <v>228</v>
@@ -2758,7 +2762,7 @@
       </c>
       <c r="F21" s="52"/>
       <c r="G21" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H21" s="53">
         <v>17</v>
@@ -2799,7 +2803,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" s="47" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>17</v>
       </c>
@@ -2807,7 +2811,7 @@
         <v>122</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D22" s="51" t="s">
         <v>228</v>
@@ -2840,7 +2844,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D23" s="51" t="s">
         <v>228</v>
@@ -2850,7 +2854,7 @@
       </c>
       <c r="F23" s="52"/>
       <c r="G23" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H23" s="53">
         <v>18</v>
@@ -2899,7 +2903,7 @@
         <v>122</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D24" s="51" t="s">
         <v>228</v>
@@ -2909,7 +2913,7 @@
       </c>
       <c r="F24" s="52"/>
       <c r="G24" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H24" s="53">
         <v>19</v>
@@ -2918,7 +2922,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K24" s="56" t="s">
         <v>20</v>
@@ -2950,7 +2954,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>17</v>
       </c>
@@ -2958,7 +2962,7 @@
         <v>122</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D25" s="51" t="s">
         <v>229</v>
@@ -2977,7 +2981,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="55" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K25" s="56" t="s">
         <v>19</v>
@@ -3003,13 +3007,13 @@
         <v>176</v>
       </c>
       <c r="T25" s="65" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="U25" s="59" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>17</v>
       </c>
@@ -3017,7 +3021,7 @@
         <v>122</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D26" s="51" t="s">
         <v>229</v>
@@ -3076,7 +3080,7 @@
         <v>122</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D27" s="51" t="s">
         <v>229</v>
@@ -3086,7 +3090,7 @@
       </c>
       <c r="F27" s="52"/>
       <c r="G27" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H27" s="53">
         <v>22</v>
@@ -3121,7 +3125,7 @@
         <v>127</v>
       </c>
       <c r="T27" s="65" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="U27" s="59" t="s">
         <v>128</v>
@@ -3135,7 +3139,7 @@
         <v>122</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D28" s="51" t="s">
         <v>229</v>
@@ -3145,7 +3149,7 @@
       </c>
       <c r="F28" s="52"/>
       <c r="G28" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H28" s="53">
         <v>23</v>
@@ -3154,7 +3158,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="55" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K28" s="56" t="s">
         <v>20</v>
@@ -3180,13 +3184,13 @@
         <v>140</v>
       </c>
       <c r="T28" s="65" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="U28" s="59" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
         <v>17</v>
       </c>
@@ -3194,7 +3198,7 @@
         <v>122</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D29" s="51" t="s">
         <v>229</v>
@@ -3204,7 +3208,7 @@
       </c>
       <c r="F29" s="52"/>
       <c r="G29" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H29" s="53">
         <v>24</v>
@@ -3245,7 +3249,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
         <v>17</v>
       </c>
@@ -3253,7 +3257,7 @@
         <v>122</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D30" s="51" t="s">
         <v>229</v>
@@ -3312,7 +3316,7 @@
         <v>122</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D31" s="51" t="s">
         <v>229</v>
@@ -3322,7 +3326,7 @@
       </c>
       <c r="F31" s="52"/>
       <c r="G31" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H31" s="53">
         <v>26</v>
@@ -3363,7 +3367,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
         <v>17</v>
       </c>
@@ -3371,7 +3375,7 @@
         <v>122</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D32" s="51" t="s">
         <v>189</v>
@@ -3420,7 +3424,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
         <v>17</v>
       </c>
@@ -3428,7 +3432,7 @@
         <v>122</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D33" s="51" t="s">
         <v>189</v>
@@ -3477,7 +3481,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
         <v>17</v>
       </c>
@@ -3485,7 +3489,7 @@
         <v>122</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D34" s="51" t="s">
         <v>189</v>
@@ -3534,13 +3538,13 @@
         <v>184</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="47" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" s="47" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48"/>
       <c r="B35" s="49" t="s">
         <v>122</v>
       </c>
       <c r="C35" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D35" s="51" t="s">
         <v>189</v>
@@ -3548,7 +3552,7 @@
       <c r="E35" s="62"/>
       <c r="F35" s="52"/>
       <c r="G35" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H35" s="53">
         <v>30</v>
@@ -3557,7 +3561,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K35" s="56" t="s">
         <v>19</v>
@@ -3583,7 +3587,7 @@
         <v>183</v>
       </c>
       <c r="T35" s="65" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U35" s="59" t="s">
         <v>184</v>
@@ -3597,7 +3601,7 @@
         <v>122</v>
       </c>
       <c r="C36" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D36" s="51" t="s">
         <v>200</v>
@@ -3642,7 +3646,7 @@
         <v>122</v>
       </c>
       <c r="C37" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D37" s="51" t="s">
         <v>200</v>
@@ -3699,7 +3703,7 @@
         <v>122</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D38" s="51" t="s">
         <v>200</v>
@@ -4716,14 +4720,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U38"/>
+  <autoFilter ref="A2:U38">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="NO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4738,6 +4742,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revisión escaleta CN 06 04
Revisión escaleta CN 06 04
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Dropbox\Editorial planeta\1. Autor\Escaletas\CN_06_04_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -519,9 +519,6 @@
     <t>La nutrición de los protistos</t>
   </si>
   <si>
-    <t>Actividad para repasar el proceso de nutrición de los protistos</t>
-  </si>
-  <si>
     <t>La nutrición de los hongos</t>
   </si>
   <si>
@@ -783,9 +780,6 @@
     <t>Los mecanismos de nutrición en microorganismos</t>
   </si>
   <si>
-    <t>La nutrición en protistos</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: La nutrición en los microorganismos</t>
   </si>
   <si>
@@ -838,6 +832,12 @@
   </si>
   <si>
     <t>Recurso M12A-01</t>
+  </si>
+  <si>
+    <t>La nutrición en protistas</t>
+  </si>
+  <si>
+    <t>Actividad para repasar el proceso de nutrición de los protistas</t>
   </si>
 </sst>
 </file>
@@ -1227,16 +1227,34 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1276,24 +1294,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1603,9 +1603,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,94 +1632,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="75" t="s">
+      <c r="G1" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="J1" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="77" t="s">
+      <c r="K1" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="75" t="s">
+      <c r="L1" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="81" t="s">
+      <c r="M1" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="81"/>
-      <c r="O1" s="69" t="s">
+      <c r="N1" s="87"/>
+      <c r="O1" s="67" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="69" t="s">
+      <c r="P1" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="84" t="s">
+      <c r="Q1" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="88" t="s">
+      <c r="R1" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="84" t="s">
+      <c r="S1" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="86" t="s">
+      <c r="T1" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="84" t="s">
+      <c r="U1" s="69" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="76"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="82"/>
       <c r="M2" s="14" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="85"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="70"/>
     </row>
     <row r="3" spans="1:21" s="47" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -1729,17 +1729,17 @@
         <v>122</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D3" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="61" t="s">
         <v>223</v>
-      </c>
-      <c r="E3" s="61" t="s">
-        <v>224</v>
       </c>
       <c r="F3" s="37"/>
       <c r="G3" s="32" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H3" s="38">
         <v>1</v>
@@ -1748,7 +1748,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K3" s="41" t="s">
         <v>20</v>
@@ -1788,17 +1788,17 @@
         <v>122</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D4" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="E4" s="62" t="s">
         <v>223</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>224</v>
       </c>
       <c r="F4" s="52"/>
       <c r="G4" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H4" s="53">
         <v>2</v>
@@ -1807,7 +1807,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K4" s="56" t="s">
         <v>20</v>
@@ -1833,7 +1833,7 @@
         <v>127</v>
       </c>
       <c r="T4" s="65" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U4" s="59" t="s">
         <v>128</v>
@@ -1847,16 +1847,16 @@
         <v>122</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E5" s="62" t="s">
         <v>132</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G5" s="31"/>
       <c r="H5" s="53"/>
@@ -1882,19 +1882,19 @@
         <v>122</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E6" s="62" t="s">
         <v>132</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H6" s="53">
         <v>3</v>
@@ -1903,7 +1903,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="55" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K6" s="56" t="s">
         <v>20</v>
@@ -1929,7 +1929,7 @@
         <v>140</v>
       </c>
       <c r="T6" s="65" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U6" s="59" t="s">
         <v>141</v>
@@ -1943,19 +1943,19 @@
         <v>122</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E7" s="62" t="s">
         <v>132</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H7" s="53">
         <v>4</v>
@@ -2004,16 +2004,16 @@
         <v>122</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E8" s="62" t="s">
         <v>132</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>131</v>
@@ -2025,7 +2025,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="55" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K8" s="56" t="s">
         <v>20</v>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="M8" s="58"/>
       <c r="N8" s="58" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="O8" s="52"/>
       <c r="P8" s="52" t="s">
@@ -2051,7 +2051,7 @@
         <v>127</v>
       </c>
       <c r="T8" s="65" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U8" s="59" t="s">
         <v>128</v>
@@ -2065,16 +2065,16 @@
         <v>122</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E9" s="62" t="s">
         <v>132</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>132</v>
@@ -2126,17 +2126,17 @@
         <v>122</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E10" s="62" t="s">
         <v>135</v>
       </c>
       <c r="F10" s="52"/>
       <c r="G10" s="31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H10" s="53">
         <v>7</v>
@@ -2145,7 +2145,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="55" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K10" s="56" t="s">
         <v>20</v>
@@ -2185,13 +2185,13 @@
         <v>122</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D11" s="51" t="s">
         <v>137</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="31" t="s">
@@ -2204,7 +2204,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="55" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K11" s="56" t="s">
         <v>20</v>
@@ -2213,7 +2213,7 @@
         <v>5</v>
       </c>
       <c r="M11" s="58" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N11" s="58"/>
       <c r="O11" s="52"/>
@@ -2230,7 +2230,7 @@
         <v>140</v>
       </c>
       <c r="T11" s="65" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U11" s="59" t="s">
         <v>141</v>
@@ -2244,13 +2244,13 @@
         <v>122</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D12" s="51" t="s">
         <v>137</v>
       </c>
       <c r="E12" s="62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F12" s="52" t="s">
         <v>142</v>
@@ -2265,7 +2265,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="55" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K12" s="56" t="s">
         <v>20</v>
@@ -2305,13 +2305,13 @@
         <v>122</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D13" s="51" t="s">
         <v>137</v>
       </c>
       <c r="E13" s="62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F13" s="52" t="s">
         <v>144</v>
@@ -2340,13 +2340,13 @@
         <v>122</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D14" s="51" t="s">
         <v>137</v>
       </c>
       <c r="E14" s="62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F14" s="52" t="s">
         <v>145</v>
@@ -2401,13 +2401,13 @@
         <v>122</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D15" s="51" t="s">
         <v>137</v>
       </c>
       <c r="E15" s="62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F15" s="52" t="s">
         <v>145</v>
@@ -2422,7 +2422,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K15" s="56" t="s">
         <v>20</v>
@@ -2448,7 +2448,7 @@
         <v>127</v>
       </c>
       <c r="T15" s="65" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="U15" s="59" t="s">
         <v>128</v>
@@ -2462,7 +2462,7 @@
         <v>122</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D16" s="51" t="s">
         <v>137</v>
@@ -2481,7 +2481,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="55" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K16" s="56" t="s">
         <v>20</v>
@@ -2521,15 +2521,15 @@
         <v>122</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E17" s="62"/>
       <c r="F17" s="52"/>
       <c r="G17" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H17" s="53">
         <v>13</v>
@@ -2564,7 +2564,7 @@
         <v>140</v>
       </c>
       <c r="T17" s="65" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="U17" s="59" t="s">
         <v>141</v>
@@ -2578,15 +2578,15 @@
         <v>122</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E18" s="62"/>
       <c r="F18" s="52"/>
       <c r="G18" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H18" s="53">
         <v>14</v>
@@ -2635,10 +2635,10 @@
         <v>122</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E19" s="62"/>
       <c r="F19" s="52"/>
@@ -2692,10 +2692,10 @@
         <v>122</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E20" s="62" t="s">
         <v>159</v>
@@ -2737,7 +2737,7 @@
         <v>127</v>
       </c>
       <c r="T20" s="65" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="U20" s="59" t="s">
         <v>128</v>
@@ -2751,17 +2751,17 @@
         <v>122</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E21" s="62" t="s">
         <v>163</v>
       </c>
       <c r="F21" s="52"/>
       <c r="G21" s="31" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="H21" s="53">
         <v>17</v>
@@ -2770,7 +2770,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="55" t="s">
-        <v>164</v>
+        <v>270</v>
       </c>
       <c r="K21" s="56" t="s">
         <v>20</v>
@@ -2810,13 +2810,13 @@
         <v>122</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E22" s="62" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F22" s="52"/>
       <c r="G22" s="31"/>
@@ -2843,17 +2843,17 @@
         <v>122</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E23" s="62" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F23" s="52"/>
       <c r="G23" s="31" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H23" s="53">
         <v>18</v>
@@ -2862,7 +2862,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="55" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K23" s="56" t="s">
         <v>20</v>
@@ -2888,7 +2888,7 @@
         <v>127</v>
       </c>
       <c r="T23" s="65" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U23" s="59" t="s">
         <v>128</v>
@@ -2902,17 +2902,17 @@
         <v>122</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E24" s="62" t="s">
         <v>135</v>
       </c>
       <c r="F24" s="52"/>
       <c r="G24" s="31" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H24" s="53">
         <v>19</v>
@@ -2921,7 +2921,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="55" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K24" s="56" t="s">
         <v>20</v>
@@ -2947,7 +2947,7 @@
         <v>127</v>
       </c>
       <c r="T24" s="65" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U24" s="59" t="s">
         <v>128</v>
@@ -2961,17 +2961,17 @@
         <v>122</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E25" s="62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F25" s="52"/>
       <c r="G25" s="31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H25" s="53">
         <v>20</v>
@@ -2980,7 +2980,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="55" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K25" s="56" t="s">
         <v>19</v>
@@ -2997,19 +2997,19 @@
         <v>19</v>
       </c>
       <c r="Q25" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="R25" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="R25" s="60" t="s">
+      <c r="S25" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="S25" s="59" t="s">
+      <c r="T25" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="U25" s="59" t="s">
         <v>176</v>
-      </c>
-      <c r="T25" s="65" t="s">
-        <v>256</v>
-      </c>
-      <c r="U25" s="59" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3020,17 +3020,17 @@
         <v>122</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D26" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E26" s="62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F26" s="52"/>
       <c r="G26" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H26" s="53">
         <v>21</v>
@@ -3039,7 +3039,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K26" s="56" t="s">
         <v>19</v>
@@ -3056,19 +3056,19 @@
         <v>19</v>
       </c>
       <c r="Q26" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="R26" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="R26" s="60" t="s">
+      <c r="S26" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="S26" s="59" t="s">
+      <c r="T26" s="65" t="s">
+        <v>171</v>
+      </c>
+      <c r="U26" s="59" t="s">
         <v>176</v>
-      </c>
-      <c r="T26" s="65" t="s">
-        <v>172</v>
-      </c>
-      <c r="U26" s="59" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3079,17 +3079,17 @@
         <v>122</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D27" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E27" s="62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F27" s="52"/>
       <c r="G27" s="31" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H27" s="53">
         <v>22</v>
@@ -3098,7 +3098,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K27" s="56" t="s">
         <v>20</v>
@@ -3124,7 +3124,7 @@
         <v>127</v>
       </c>
       <c r="T27" s="65" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="U27" s="59" t="s">
         <v>128</v>
@@ -3138,17 +3138,17 @@
         <v>122</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D28" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E28" s="62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F28" s="52"/>
       <c r="G28" s="31" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H28" s="53">
         <v>23</v>
@@ -3157,7 +3157,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="55" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K28" s="56" t="s">
         <v>20</v>
@@ -3183,7 +3183,7 @@
         <v>140</v>
       </c>
       <c r="T28" s="65" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="U28" s="59" t="s">
         <v>141</v>
@@ -3197,17 +3197,17 @@
         <v>122</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D29" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F29" s="52"/>
       <c r="G29" s="31" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H29" s="53">
         <v>24</v>
@@ -3216,7 +3216,7 @@
         <v>19</v>
       </c>
       <c r="J29" s="55" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K29" s="56" t="s">
         <v>19</v>
@@ -3233,19 +3233,19 @@
         <v>19</v>
       </c>
       <c r="Q29" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="R29" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="R29" s="60" t="s">
-        <v>175</v>
-      </c>
       <c r="S29" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="T29" s="65" t="s">
+        <v>180</v>
+      </c>
+      <c r="U29" s="59" t="s">
         <v>183</v>
-      </c>
-      <c r="T29" s="65" t="s">
-        <v>181</v>
-      </c>
-      <c r="U29" s="59" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3256,17 +3256,17 @@
         <v>122</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D30" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E30" s="62" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F30" s="52"/>
       <c r="G30" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H30" s="53">
         <v>25</v>
@@ -3275,7 +3275,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="55" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K30" s="56" t="s">
         <v>19</v>
@@ -3292,19 +3292,19 @@
         <v>19</v>
       </c>
       <c r="Q30" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="R30" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="R30" s="60" t="s">
-        <v>175</v>
-      </c>
       <c r="S30" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="T30" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="U30" s="59" t="s">
         <v>183</v>
-      </c>
-      <c r="T30" s="65" t="s">
-        <v>185</v>
-      </c>
-      <c r="U30" s="59" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3315,17 +3315,17 @@
         <v>122</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E31" s="62" t="s">
         <v>135</v>
       </c>
       <c r="F31" s="52"/>
       <c r="G31" s="31" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H31" s="53">
         <v>26</v>
@@ -3334,7 +3334,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="55" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K31" s="56" t="s">
         <v>20</v>
@@ -3360,7 +3360,7 @@
         <v>127</v>
       </c>
       <c r="T31" s="65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U31" s="59" t="s">
         <v>128</v>
@@ -3374,15 +3374,15 @@
         <v>122</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D32" s="51" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E32" s="62"/>
       <c r="F32" s="52"/>
       <c r="G32" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H32" s="53">
         <v>27</v>
@@ -3391,7 +3391,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K32" s="56" t="s">
         <v>19</v>
@@ -3401,26 +3401,26 @@
       </c>
       <c r="M32" s="58"/>
       <c r="N32" s="58" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O32" s="52"/>
       <c r="P32" s="52" t="s">
         <v>19</v>
       </c>
       <c r="Q32" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="R32" s="60" t="s">
+        <v>174</v>
+      </c>
+      <c r="S32" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="R32" s="60" t="s">
-        <v>175</v>
-      </c>
-      <c r="S32" s="59" t="s">
+      <c r="T32" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="U32" s="59" t="s">
         <v>194</v>
-      </c>
-      <c r="T32" s="65" t="s">
-        <v>190</v>
-      </c>
-      <c r="U32" s="59" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3431,15 +3431,15 @@
         <v>122</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E33" s="62"/>
       <c r="F33" s="52"/>
       <c r="G33" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H33" s="53">
         <v>28</v>
@@ -3448,7 +3448,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="55" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K33" s="56" t="s">
         <v>19</v>
@@ -3458,26 +3458,26 @@
       </c>
       <c r="M33" s="58"/>
       <c r="N33" s="58" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O33" s="52"/>
       <c r="P33" s="52" t="s">
         <v>19</v>
       </c>
       <c r="Q33" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="R33" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="R33" s="60" t="s">
+      <c r="S33" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="S33" s="59" t="s">
+      <c r="T33" s="65" t="s">
+        <v>195</v>
+      </c>
+      <c r="U33" s="59" t="s">
         <v>176</v>
-      </c>
-      <c r="T33" s="65" t="s">
-        <v>196</v>
-      </c>
-      <c r="U33" s="59" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3488,15 +3488,15 @@
         <v>122</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D34" s="51" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E34" s="62"/>
       <c r="F34" s="52"/>
       <c r="G34" s="31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H34" s="53">
         <v>29</v>
@@ -3505,7 +3505,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="55" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K34" s="56" t="s">
         <v>19</v>
@@ -3515,26 +3515,26 @@
       </c>
       <c r="M34" s="58"/>
       <c r="N34" s="58" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O34" s="52"/>
       <c r="P34" s="52" t="s">
         <v>19</v>
       </c>
       <c r="Q34" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="R34" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="R34" s="60" t="s">
-        <v>175</v>
-      </c>
       <c r="S34" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="T34" s="65" t="s">
+        <v>197</v>
+      </c>
+      <c r="U34" s="59" t="s">
         <v>183</v>
-      </c>
-      <c r="T34" s="65" t="s">
-        <v>198</v>
-      </c>
-      <c r="U34" s="59" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:21" s="47" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3543,15 +3543,15 @@
         <v>122</v>
       </c>
       <c r="C35" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D35" s="51" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E35" s="62"/>
       <c r="F35" s="52"/>
       <c r="G35" s="31" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H35" s="53">
         <v>30</v>
@@ -3560,7 +3560,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="55" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K35" s="56" t="s">
         <v>19</v>
@@ -3570,26 +3570,26 @@
       </c>
       <c r="M35" s="58"/>
       <c r="N35" s="58" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O35" s="52"/>
       <c r="P35" s="52" t="s">
         <v>19</v>
       </c>
       <c r="Q35" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="R35" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="R35" s="60" t="s">
-        <v>175</v>
-      </c>
       <c r="S35" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="T35" s="65" t="s">
+        <v>260</v>
+      </c>
+      <c r="U35" s="59" t="s">
         <v>183</v>
-      </c>
-      <c r="T35" s="65" t="s">
-        <v>262</v>
-      </c>
-      <c r="U35" s="59" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -3600,15 +3600,15 @@
         <v>122</v>
       </c>
       <c r="C36" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D36" s="51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E36" s="62"/>
       <c r="F36" s="52"/>
       <c r="G36" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H36" s="53">
         <v>31</v>
@@ -3617,7 +3617,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="55" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K36" s="56" t="s">
         <v>20</v>
@@ -3645,15 +3645,15 @@
         <v>122</v>
       </c>
       <c r="C37" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D37" s="51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E37" s="62"/>
       <c r="F37" s="52"/>
       <c r="G37" s="31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H37" s="53">
         <v>32</v>
@@ -3662,7 +3662,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="55" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K37" s="56" t="s">
         <v>20</v>
@@ -3688,7 +3688,7 @@
         <v>127</v>
       </c>
       <c r="T37" s="65" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U37" s="59" t="s">
         <v>128</v>
@@ -3702,24 +3702,24 @@
         <v>122</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D38" s="51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E38" s="62"/>
       <c r="F38" s="52"/>
       <c r="G38" s="31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H38" s="53">
         <v>33</v>
       </c>
       <c r="I38" s="54" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J38" s="55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K38" s="56" t="s">
         <v>20</v>
@@ -3745,7 +3745,7 @@
         <v>127</v>
       </c>
       <c r="T38" s="65" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U38" s="59" t="s">
         <v>128</v>
@@ -4721,12 +4721,6 @@
   </sheetData>
   <autoFilter ref="A2:U38"/>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4741,6 +4735,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4802,19 +4802,19 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="21" t="s">
         <v>212</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4824,7 +4824,7 @@
       <c r="B3" s="23"/>
       <c r="C3" s="24"/>
       <c r="D3" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" s="26"/>
     </row>
@@ -4837,7 +4837,7 @@
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E4" s="26"/>
     </row>
@@ -4846,70 +4846,70 @@
         <v>152</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="D8" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="D9" s="28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E9" s="29"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
       <c r="D10" s="28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E10" s="29"/>
     </row>

</xml_diff>

<commit_message>
Actualización escaleta y mapa CN 06 04
Actualización escaleta y mapa CN 06 04
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion04/Escaleta CN_06_04_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Dropbox\Editorial planeta\1. Autor\Escaletas\CN_06_04_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,14 +17,14 @@
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Escaleta!$A$2:$U$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Escaleta!$A$2:$U$39</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="274">
   <si>
     <t>Asignatura</t>
   </si>
@@ -717,9 +717,6 @@
     <t>Actividad acerca del concepto de la nutrición</t>
   </si>
   <si>
-    <t>Actividad para reforzar los conocimientos sobre la cadena trófica</t>
-  </si>
-  <si>
     <t>F6B</t>
   </si>
   <si>
@@ -844,6 +841,12 @@
   </si>
   <si>
     <t>Relaciona conceptos de la nutrición en bacterias y arqueas</t>
+  </si>
+  <si>
+    <t>Reconoce la cadena alimenticia</t>
+  </si>
+  <si>
+    <t>Actividad para reforzar los conocimientos sobre la cadena alimenticia</t>
   </si>
 </sst>
 </file>
@@ -1607,11 +1610,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U123"/>
+  <dimension ref="A1:U124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A2"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,7 +1738,7 @@
         <v>122</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>213</v>
@@ -1745,7 +1748,7 @@
       </c>
       <c r="F3" s="37"/>
       <c r="G3" s="32" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H3" s="38">
         <v>1</v>
@@ -1794,7 +1797,7 @@
         <v>122</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D4" s="51" t="s">
         <v>213</v>
@@ -1853,7 +1856,7 @@
         <v>122</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D5" s="51" t="s">
         <v>213</v>
@@ -1880,7 +1883,7 @@
       <c r="T5" s="65"/>
       <c r="U5" s="59"/>
     </row>
-    <row r="6" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>17</v>
       </c>
@@ -1888,7 +1891,7 @@
         <v>122</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D6" s="51" t="s">
         <v>213</v>
@@ -1899,47 +1902,21 @@
       <c r="F6" s="52" t="s">
         <v>216</v>
       </c>
-      <c r="G6" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="H6" s="53">
-        <v>3</v>
-      </c>
-      <c r="I6" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="55" t="s">
-        <v>226</v>
-      </c>
-      <c r="K6" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="57" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="58" t="s">
-        <v>53</v>
-      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="58"/>
       <c r="N6" s="58"/>
       <c r="O6" s="52"/>
-      <c r="P6" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="59">
-        <v>6</v>
-      </c>
-      <c r="R6" s="60" t="s">
-        <v>139</v>
-      </c>
-      <c r="S6" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="T6" s="65" t="s">
-        <v>225</v>
-      </c>
-      <c r="U6" s="59" t="s">
-        <v>141</v>
-      </c>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="60"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="65"/>
+      <c r="U6" s="59"/>
     </row>
     <row r="7" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -1949,7 +1926,7 @@
         <v>122</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D7" s="51" t="s">
         <v>213</v>
@@ -1958,30 +1935,30 @@
         <v>132</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>216</v>
+        <v>131</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="H7" s="53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I7" s="54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" s="55" t="s">
-        <v>129</v>
+        <v>226</v>
       </c>
       <c r="K7" s="56" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58" t="s">
-        <v>44</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="M7" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="58"/>
       <c r="O7" s="52"/>
       <c r="P7" s="52" t="s">
         <v>19</v>
@@ -1990,19 +1967,19 @@
         <v>6</v>
       </c>
       <c r="R7" s="60" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="S7" s="59" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="T7" s="65" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
       <c r="U7" s="59" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>17</v>
       </c>
@@ -2010,7 +1987,7 @@
         <v>122</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D8" s="51" t="s">
         <v>213</v>
@@ -2019,19 +1996,19 @@
         <v>132</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>216</v>
+        <v>131</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>131</v>
+        <v>224</v>
       </c>
       <c r="H8" s="53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="55" t="s">
-        <v>230</v>
+        <v>129</v>
       </c>
       <c r="K8" s="56" t="s">
         <v>20</v>
@@ -2041,7 +2018,7 @@
       </c>
       <c r="M8" s="58"/>
       <c r="N8" s="58" t="s">
-        <v>254</v>
+        <v>44</v>
       </c>
       <c r="O8" s="52"/>
       <c r="P8" s="52" t="s">
@@ -2057,7 +2034,7 @@
         <v>127</v>
       </c>
       <c r="T8" s="65" t="s">
-        <v>255</v>
+        <v>130</v>
       </c>
       <c r="U8" s="59" t="s">
         <v>128</v>
@@ -2071,7 +2048,7 @@
         <v>122</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D9" s="51" t="s">
         <v>213</v>
@@ -2080,19 +2057,19 @@
         <v>132</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>216</v>
+        <v>131</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="H9" s="53">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I9" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>133</v>
+        <v>273</v>
       </c>
       <c r="K9" s="56" t="s">
         <v>20</v>
@@ -2102,11 +2079,11 @@
       </c>
       <c r="M9" s="58"/>
       <c r="N9" s="58" t="s">
-        <v>32</v>
+        <v>253</v>
       </c>
       <c r="O9" s="52"/>
-      <c r="P9" s="30" t="s">
-        <v>20</v>
+      <c r="P9" s="52" t="s">
+        <v>19</v>
       </c>
       <c r="Q9" s="59">
         <v>6</v>
@@ -2118,7 +2095,7 @@
         <v>127</v>
       </c>
       <c r="T9" s="65" t="s">
-        <v>134</v>
+        <v>254</v>
       </c>
       <c r="U9" s="59" t="s">
         <v>128</v>
@@ -2132,26 +2109,28 @@
         <v>122</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D10" s="51" t="s">
         <v>213</v>
       </c>
       <c r="E10" s="62" t="s">
-        <v>135</v>
-      </c>
-      <c r="F10" s="52"/>
+        <v>132</v>
+      </c>
+      <c r="F10" s="52" t="s">
+        <v>131</v>
+      </c>
       <c r="G10" s="31" t="s">
-        <v>220</v>
+        <v>266</v>
       </c>
       <c r="H10" s="53">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I10" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J10" s="55" t="s">
-        <v>229</v>
+        <v>133</v>
       </c>
       <c r="K10" s="56" t="s">
         <v>20</v>
@@ -2161,11 +2140,11 @@
       </c>
       <c r="M10" s="58"/>
       <c r="N10" s="58" t="s">
-        <v>121</v>
+        <v>32</v>
       </c>
       <c r="O10" s="52"/>
-      <c r="P10" s="52" t="s">
-        <v>19</v>
+      <c r="P10" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="Q10" s="59">
         <v>6</v>
@@ -2177,7 +2156,7 @@
         <v>127</v>
       </c>
       <c r="T10" s="65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="U10" s="59" t="s">
         <v>128</v>
@@ -2191,37 +2170,37 @@
         <v>122</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>137</v>
+        <v>213</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>217</v>
+        <v>135</v>
       </c>
       <c r="F11" s="52"/>
       <c r="G11" s="31" t="s">
-        <v>138</v>
+        <v>220</v>
       </c>
       <c r="H11" s="53">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I11" s="54" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J11" s="55" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="K11" s="56" t="s">
         <v>20</v>
       </c>
       <c r="L11" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="M11" s="58" t="s">
-        <v>231</v>
-      </c>
-      <c r="N11" s="58"/>
+        <v>8</v>
+      </c>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58" t="s">
+        <v>121</v>
+      </c>
       <c r="O11" s="52"/>
       <c r="P11" s="52" t="s">
         <v>19</v>
@@ -2230,16 +2209,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="60" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="S11" s="59" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="T11" s="65" t="s">
-        <v>232</v>
+        <v>136</v>
       </c>
       <c r="U11" s="59" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2250,7 +2229,7 @@
         <v>122</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D12" s="51" t="s">
         <v>137</v>
@@ -2258,31 +2237,29 @@
       <c r="E12" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="F12" s="52" t="s">
-        <v>142</v>
-      </c>
+      <c r="F12" s="52"/>
       <c r="G12" s="31" t="s">
-        <v>271</v>
+        <v>138</v>
       </c>
       <c r="H12" s="53">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I12" s="54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12" s="55" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K12" s="56" t="s">
         <v>20</v>
       </c>
       <c r="L12" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58" t="s">
-        <v>23</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M12" s="58" t="s">
+        <v>230</v>
+      </c>
+      <c r="N12" s="58"/>
       <c r="O12" s="52"/>
       <c r="P12" s="52" t="s">
         <v>19</v>
@@ -2291,16 +2268,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="60" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="S12" s="59" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="T12" s="65" t="s">
-        <v>158</v>
+        <v>231</v>
       </c>
       <c r="U12" s="59" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2311,7 +2288,7 @@
         <v>122</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D13" s="51" t="s">
         <v>137</v>
@@ -2320,23 +2297,49 @@
         <v>217</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>144</v>
-      </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="57"/>
+        <v>142</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="H13" s="53">
+        <v>9</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="K13" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="57" t="s">
+        <v>8</v>
+      </c>
       <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
+      <c r="N13" s="58" t="s">
+        <v>23</v>
+      </c>
       <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="59"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="65"/>
-      <c r="U13" s="59"/>
+      <c r="P13" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="59">
+        <v>6</v>
+      </c>
+      <c r="R13" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="S13" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T13" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="U13" s="59" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="14" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
@@ -2346,7 +2349,7 @@
         <v>122</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D14" s="51" t="s">
         <v>137</v>
@@ -2355,49 +2358,23 @@
         <v>217</v>
       </c>
       <c r="F14" s="52" t="s">
-        <v>145</v>
-      </c>
-      <c r="G14" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="H14" s="53">
-        <v>10</v>
-      </c>
-      <c r="I14" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="55" t="s">
-        <v>147</v>
-      </c>
-      <c r="K14" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="57" t="s">
-        <v>8</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="G14" s="31"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="57"/>
       <c r="M14" s="58"/>
-      <c r="N14" s="58" t="s">
-        <v>43</v>
-      </c>
+      <c r="N14" s="58"/>
       <c r="O14" s="52"/>
-      <c r="P14" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="59">
-        <v>6</v>
-      </c>
-      <c r="R14" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="S14" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="T14" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="U14" s="59" t="s">
-        <v>128</v>
-      </c>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="59"/>
+      <c r="R14" s="60"/>
+      <c r="S14" s="59"/>
+      <c r="T14" s="65"/>
+      <c r="U14" s="59"/>
     </row>
     <row r="15" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
@@ -2407,7 +2384,7 @@
         <v>122</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D15" s="51" t="s">
         <v>137</v>
@@ -2419,16 +2396,16 @@
         <v>145</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>268</v>
+        <v>146</v>
       </c>
       <c r="H15" s="53">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I15" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>236</v>
+        <v>147</v>
       </c>
       <c r="K15" s="56" t="s">
         <v>20</v>
@@ -2438,7 +2415,7 @@
       </c>
       <c r="M15" s="58"/>
       <c r="N15" s="58" t="s">
-        <v>119</v>
+        <v>43</v>
       </c>
       <c r="O15" s="52"/>
       <c r="P15" s="52" t="s">
@@ -2454,13 +2431,13 @@
         <v>127</v>
       </c>
       <c r="T15" s="65" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="U15" s="59" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>17</v>
       </c>
@@ -2468,26 +2445,28 @@
         <v>122</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D16" s="51" t="s">
         <v>137</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>135</v>
-      </c>
-      <c r="F16" s="52"/>
+        <v>217</v>
+      </c>
+      <c r="F16" s="52" t="s">
+        <v>145</v>
+      </c>
       <c r="G16" s="31" t="s">
-        <v>149</v>
+        <v>267</v>
       </c>
       <c r="H16" s="53">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I16" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K16" s="56" t="s">
         <v>20</v>
@@ -2497,7 +2476,7 @@
       </c>
       <c r="M16" s="58"/>
       <c r="N16" s="58" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O16" s="52"/>
       <c r="P16" s="52" t="s">
@@ -2513,13 +2492,13 @@
         <v>127</v>
       </c>
       <c r="T16" s="65" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="U16" s="59" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
         <v>17</v>
       </c>
@@ -2527,35 +2506,37 @@
         <v>122</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>218</v>
-      </c>
-      <c r="E17" s="62"/>
+        <v>137</v>
+      </c>
+      <c r="E17" s="62" t="s">
+        <v>135</v>
+      </c>
       <c r="F17" s="52"/>
       <c r="G17" s="31" t="s">
-        <v>238</v>
+        <v>149</v>
       </c>
       <c r="H17" s="53">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I17" s="54" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J17" s="55" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="K17" s="56" t="s">
         <v>20</v>
       </c>
       <c r="L17" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="M17" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="N17" s="58"/>
+        <v>8</v>
+      </c>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58" t="s">
+        <v>121</v>
+      </c>
       <c r="O17" s="52"/>
       <c r="P17" s="52" t="s">
         <v>19</v>
@@ -2564,16 +2545,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="60" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="S17" s="59" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="T17" s="65" t="s">
-        <v>239</v>
+        <v>150</v>
       </c>
       <c r="U17" s="59" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2584,7 +2565,7 @@
         <v>122</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D18" s="51" t="s">
         <v>218</v>
@@ -2592,27 +2573,27 @@
       <c r="E18" s="62"/>
       <c r="F18" s="52"/>
       <c r="G18" s="31" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H18" s="53">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I18" s="54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" s="55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K18" s="56" t="s">
         <v>20</v>
       </c>
       <c r="L18" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58" t="s">
-        <v>51</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M18" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="N18" s="58"/>
       <c r="O18" s="52"/>
       <c r="P18" s="52" t="s">
         <v>19</v>
@@ -2621,16 +2602,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="60" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="S18" s="59" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="T18" s="65" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="U18" s="59" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2641,7 +2622,7 @@
         <v>122</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D19" s="51" t="s">
         <v>218</v>
@@ -2649,16 +2630,16 @@
       <c r="E19" s="62"/>
       <c r="F19" s="52"/>
       <c r="G19" s="31" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H19" s="53">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I19" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="55" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K19" s="56" t="s">
         <v>20</v>
@@ -2668,7 +2649,7 @@
       </c>
       <c r="M19" s="58"/>
       <c r="N19" s="58" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="O19" s="52"/>
       <c r="P19" s="52" t="s">
@@ -2684,7 +2665,7 @@
         <v>127</v>
       </c>
       <c r="T19" s="65" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="U19" s="59" t="s">
         <v>128</v>
@@ -2698,26 +2679,24 @@
         <v>122</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D20" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="E20" s="62" t="s">
-        <v>157</v>
-      </c>
+      <c r="E20" s="62"/>
       <c r="F20" s="52"/>
       <c r="G20" s="31" t="s">
-        <v>272</v>
+        <v>241</v>
       </c>
       <c r="H20" s="53">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I20" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J20" s="55" t="s">
-        <v>257</v>
+        <v>155</v>
       </c>
       <c r="K20" s="56" t="s">
         <v>20</v>
@@ -2727,7 +2706,7 @@
       </c>
       <c r="M20" s="58"/>
       <c r="N20" s="58" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O20" s="52"/>
       <c r="P20" s="52" t="s">
@@ -2743,13 +2722,13 @@
         <v>127</v>
       </c>
       <c r="T20" s="65" t="s">
-        <v>235</v>
+        <v>156</v>
       </c>
       <c r="U20" s="59" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
         <v>17</v>
       </c>
@@ -2757,20 +2736,20 @@
         <v>122</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D21" s="51" t="s">
         <v>218</v>
       </c>
       <c r="E21" s="62" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F21" s="52"/>
       <c r="G21" s="31" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H21" s="53">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I21" s="54" t="s">
         <v>20</v>
@@ -2786,7 +2765,7 @@
       </c>
       <c r="M21" s="58"/>
       <c r="N21" s="58" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="O21" s="52"/>
       <c r="P21" s="52" t="s">
@@ -2802,7 +2781,7 @@
         <v>127</v>
       </c>
       <c r="T21" s="65" t="s">
-        <v>143</v>
+        <v>234</v>
       </c>
       <c r="U21" s="59" t="s">
         <v>128</v>
@@ -2816,32 +2795,58 @@
         <v>122</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D22" s="51" t="s">
         <v>218</v>
       </c>
       <c r="E22" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F22" s="52"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="57"/>
+      <c r="G22" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="H22" s="53">
+        <v>17</v>
+      </c>
+      <c r="I22" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="55" t="s">
+        <v>255</v>
+      </c>
+      <c r="K22" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="57" t="s">
+        <v>8</v>
+      </c>
       <c r="M22" s="58"/>
-      <c r="N22" s="58"/>
+      <c r="N22" s="58" t="s">
+        <v>27</v>
+      </c>
       <c r="O22" s="52"/>
-      <c r="P22" s="52"/>
-      <c r="Q22" s="59"/>
-      <c r="R22" s="60"/>
-      <c r="S22" s="59"/>
-      <c r="T22" s="65"/>
-      <c r="U22" s="59"/>
-    </row>
-    <row r="23" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="P22" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="59">
+        <v>6</v>
+      </c>
+      <c r="R22" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="S22" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T22" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="U22" s="59" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>17</v>
       </c>
@@ -2849,7 +2854,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D23" s="51" t="s">
         <v>218</v>
@@ -2858,47 +2863,21 @@
         <v>160</v>
       </c>
       <c r="F23" s="52"/>
-      <c r="G23" s="31" t="s">
-        <v>270</v>
-      </c>
-      <c r="H23" s="53">
-        <v>18</v>
-      </c>
-      <c r="I23" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="55" t="s">
-        <v>161</v>
-      </c>
-      <c r="K23" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="57" t="s">
-        <v>8</v>
-      </c>
+      <c r="G23" s="31"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="57"/>
       <c r="M23" s="58"/>
-      <c r="N23" s="58" t="s">
-        <v>32</v>
-      </c>
+      <c r="N23" s="58"/>
       <c r="O23" s="52"/>
-      <c r="P23" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q23" s="59">
-        <v>6</v>
-      </c>
-      <c r="R23" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="S23" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="T23" s="65" t="s">
-        <v>162</v>
-      </c>
-      <c r="U23" s="59" t="s">
-        <v>128</v>
-      </c>
+      <c r="P23" s="52"/>
+      <c r="Q23" s="59"/>
+      <c r="R23" s="60"/>
+      <c r="S23" s="59"/>
+      <c r="T23" s="65"/>
+      <c r="U23" s="59"/>
     </row>
     <row r="24" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
@@ -2908,26 +2887,26 @@
         <v>122</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D24" s="51" t="s">
         <v>218</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="F24" s="52"/>
       <c r="G24" s="31" t="s">
-        <v>241</v>
+        <v>269</v>
       </c>
       <c r="H24" s="53">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I24" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J24" s="55" t="s">
-        <v>243</v>
+        <v>161</v>
       </c>
       <c r="K24" s="56" t="s">
         <v>20</v>
@@ -2937,7 +2916,7 @@
       </c>
       <c r="M24" s="58"/>
       <c r="N24" s="58" t="s">
-        <v>121</v>
+        <v>32</v>
       </c>
       <c r="O24" s="52"/>
       <c r="P24" s="52" t="s">
@@ -2953,7 +2932,7 @@
         <v>127</v>
       </c>
       <c r="T24" s="65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U24" s="59" t="s">
         <v>128</v>
@@ -2967,55 +2946,55 @@
         <v>122</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E25" s="62" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="F25" s="52"/>
       <c r="G25" s="31" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="H25" s="53">
+        <v>19</v>
+      </c>
+      <c r="I25" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="54" t="s">
-        <v>19</v>
-      </c>
       <c r="J25" s="55" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="K25" s="56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L25" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="M25" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="N25" s="58"/>
+        <v>8</v>
+      </c>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58" t="s">
+        <v>121</v>
+      </c>
       <c r="O25" s="52"/>
       <c r="P25" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="59" t="s">
-        <v>169</v>
+      <c r="Q25" s="59">
+        <v>6</v>
       </c>
       <c r="R25" s="60" t="s">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="S25" s="59" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="T25" s="65" t="s">
-        <v>244</v>
+        <v>163</v>
       </c>
       <c r="U25" s="59" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3026,7 +3005,7 @@
         <v>122</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D26" s="51" t="s">
         <v>219</v>
@@ -3036,27 +3015,27 @@
       </c>
       <c r="F26" s="52"/>
       <c r="G26" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H26" s="53">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I26" s="54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J26" s="55" t="s">
-        <v>168</v>
+        <v>257</v>
       </c>
       <c r="K26" s="56" t="s">
         <v>19</v>
       </c>
       <c r="L26" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58" t="s">
-        <v>45</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M26" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="N26" s="58"/>
       <c r="O26" s="52"/>
       <c r="P26" s="52" t="s">
         <v>19</v>
@@ -3071,7 +3050,7 @@
         <v>171</v>
       </c>
       <c r="T26" s="65" t="s">
-        <v>167</v>
+        <v>243</v>
       </c>
       <c r="U26" s="59" t="s">
         <v>172</v>
@@ -3085,7 +3064,7 @@
         <v>122</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D27" s="51" t="s">
         <v>219</v>
@@ -3095,45 +3074,45 @@
       </c>
       <c r="F27" s="52"/>
       <c r="G27" s="31" t="s">
-        <v>246</v>
+        <v>167</v>
       </c>
       <c r="H27" s="53">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I27" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J27" s="55" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K27" s="56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L27" s="57" t="s">
         <v>8</v>
       </c>
       <c r="M27" s="58"/>
       <c r="N27" s="58" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
       <c r="O27" s="52"/>
       <c r="P27" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="59">
-        <v>6</v>
+      <c r="Q27" s="59" t="s">
+        <v>169</v>
       </c>
       <c r="R27" s="60" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="S27" s="59" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="T27" s="65" t="s">
-        <v>245</v>
+        <v>167</v>
       </c>
       <c r="U27" s="59" t="s">
-        <v>128</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3144,7 +3123,7 @@
         <v>122</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D28" s="51" t="s">
         <v>219</v>
@@ -3154,27 +3133,27 @@
       </c>
       <c r="F28" s="52"/>
       <c r="G28" s="31" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H28" s="53">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I28" s="54" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J28" s="55" t="s">
-        <v>259</v>
+        <v>173</v>
       </c>
       <c r="K28" s="56" t="s">
         <v>20</v>
       </c>
       <c r="L28" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="M28" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="N28" s="58"/>
+        <v>8</v>
+      </c>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58" t="s">
+        <v>119</v>
+      </c>
       <c r="O28" s="52"/>
       <c r="P28" s="52" t="s">
         <v>19</v>
@@ -3183,16 +3162,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="60" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="S28" s="59" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="T28" s="65" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="U28" s="59" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3203,55 +3182,55 @@
         <v>122</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D29" s="51" t="s">
         <v>219</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F29" s="52"/>
       <c r="G29" s="31" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="H29" s="53">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I29" s="54" t="s">
         <v>19</v>
       </c>
       <c r="J29" s="55" t="s">
-        <v>177</v>
+        <v>258</v>
       </c>
       <c r="K29" s="56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L29" s="57" t="s">
         <v>5</v>
       </c>
       <c r="M29" s="58" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="N29" s="58"/>
       <c r="O29" s="52"/>
       <c r="P29" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="59" t="s">
-        <v>169</v>
+      <c r="Q29" s="59">
+        <v>6</v>
       </c>
       <c r="R29" s="60" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="S29" s="59" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="T29" s="65" t="s">
-        <v>176</v>
+        <v>250</v>
       </c>
       <c r="U29" s="59" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3262,7 +3241,7 @@
         <v>122</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D30" s="51" t="s">
         <v>219</v>
@@ -3272,27 +3251,27 @@
       </c>
       <c r="F30" s="52"/>
       <c r="G30" s="31" t="s">
-        <v>180</v>
+        <v>246</v>
       </c>
       <c r="H30" s="53">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I30" s="54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J30" s="55" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="K30" s="56" t="s">
         <v>19</v>
       </c>
       <c r="L30" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58" t="s">
-        <v>23</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M30" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" s="58"/>
       <c r="O30" s="52"/>
       <c r="P30" s="52" t="s">
         <v>19</v>
@@ -3307,7 +3286,7 @@
         <v>178</v>
       </c>
       <c r="T30" s="65" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="U30" s="59" t="s">
         <v>179</v>
@@ -3321,55 +3300,55 @@
         <v>122</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D31" s="51" t="s">
         <v>219</v>
       </c>
       <c r="E31" s="62" t="s">
-        <v>135</v>
+        <v>175</v>
       </c>
       <c r="F31" s="52"/>
       <c r="G31" s="31" t="s">
-        <v>248</v>
+        <v>180</v>
       </c>
       <c r="H31" s="53">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I31" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J31" s="55" t="s">
-        <v>265</v>
+        <v>181</v>
       </c>
       <c r="K31" s="56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L31" s="57" t="s">
         <v>8</v>
       </c>
       <c r="M31" s="58"/>
       <c r="N31" s="58" t="s">
-        <v>121</v>
+        <v>23</v>
       </c>
       <c r="O31" s="52"/>
       <c r="P31" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="59">
-        <v>6</v>
+      <c r="Q31" s="59" t="s">
+        <v>169</v>
       </c>
       <c r="R31" s="60" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="S31" s="59" t="s">
-        <v>127</v>
+        <v>178</v>
       </c>
       <c r="T31" s="65" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="U31" s="59" t="s">
-        <v>128</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3380,53 +3359,55 @@
         <v>122</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D32" s="51" t="s">
-        <v>183</v>
-      </c>
-      <c r="E32" s="62"/>
+        <v>219</v>
+      </c>
+      <c r="E32" s="62" t="s">
+        <v>135</v>
+      </c>
       <c r="F32" s="52"/>
       <c r="G32" s="31" t="s">
-        <v>184</v>
+        <v>247</v>
       </c>
       <c r="H32" s="53">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I32" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J32" s="55" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="K32" s="56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L32" s="57" t="s">
         <v>8</v>
       </c>
       <c r="M32" s="58"/>
       <c r="N32" s="58" t="s">
-        <v>185</v>
+        <v>121</v>
       </c>
       <c r="O32" s="52"/>
       <c r="P32" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="59" t="s">
-        <v>186</v>
+      <c r="Q32" s="59">
+        <v>6</v>
       </c>
       <c r="R32" s="60" t="s">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="S32" s="59" t="s">
-        <v>187</v>
+        <v>127</v>
       </c>
       <c r="T32" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="U32" s="59" t="s">
-        <v>188</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3437,7 +3418,7 @@
         <v>122</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D33" s="51" t="s">
         <v>183</v>
@@ -3445,16 +3426,16 @@
       <c r="E33" s="62"/>
       <c r="F33" s="52"/>
       <c r="G33" s="31" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="H33" s="53">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I33" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J33" s="55" t="s">
-        <v>190</v>
+        <v>259</v>
       </c>
       <c r="K33" s="56" t="s">
         <v>19</v>
@@ -3471,19 +3452,19 @@
         <v>19</v>
       </c>
       <c r="Q33" s="59" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="R33" s="60" t="s">
         <v>170</v>
       </c>
       <c r="S33" s="59" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="T33" s="65" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="U33" s="59" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3494,7 +3475,7 @@
         <v>122</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D34" s="51" t="s">
         <v>183</v>
@@ -3502,16 +3483,16 @@
       <c r="E34" s="62"/>
       <c r="F34" s="52"/>
       <c r="G34" s="31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H34" s="53">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I34" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J34" s="55" t="s">
-        <v>261</v>
+        <v>190</v>
       </c>
       <c r="K34" s="56" t="s">
         <v>19</v>
@@ -3534,22 +3515,24 @@
         <v>170</v>
       </c>
       <c r="S34" s="59" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="T34" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="U34" s="59" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" s="47" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="48" t="s">
+        <v>17</v>
+      </c>
       <c r="B35" s="49" t="s">
         <v>122</v>
       </c>
       <c r="C35" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D35" s="51" t="s">
         <v>183</v>
@@ -3557,16 +3540,16 @@
       <c r="E35" s="62"/>
       <c r="F35" s="52"/>
       <c r="G35" s="31" t="s">
-        <v>249</v>
+        <v>191</v>
       </c>
       <c r="H35" s="53">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I35" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J35" s="55" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="K35" s="56" t="s">
         <v>19</v>
@@ -3592,58 +3575,68 @@
         <v>178</v>
       </c>
       <c r="T35" s="65" t="s">
-        <v>249</v>
+        <v>191</v>
       </c>
       <c r="U35" s="59" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="48" t="s">
-        <v>17</v>
-      </c>
+    <row r="36" spans="1:21" s="47" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="48"/>
       <c r="B36" s="49" t="s">
         <v>122</v>
       </c>
       <c r="C36" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D36" s="51" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="E36" s="62"/>
       <c r="F36" s="52"/>
       <c r="G36" s="31" t="s">
-        <v>193</v>
+        <v>248</v>
       </c>
       <c r="H36" s="53">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I36" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J36" s="55" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="K36" s="56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L36" s="57" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M36" s="58"/>
-      <c r="N36" s="58"/>
+      <c r="N36" s="58" t="s">
+        <v>185</v>
+      </c>
       <c r="O36" s="52"/>
       <c r="P36" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q36" s="59"/>
-      <c r="R36" s="60"/>
-      <c r="S36" s="59"/>
-      <c r="T36" s="65"/>
-      <c r="U36" s="59"/>
-    </row>
-    <row r="37" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q36" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="R36" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="S36" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="T36" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="U36" s="59" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
         <v>17</v>
       </c>
@@ -3651,7 +3644,7 @@
         <v>122</v>
       </c>
       <c r="C37" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D37" s="51" t="s">
         <v>192</v>
@@ -3659,48 +3652,36 @@
       <c r="E37" s="62"/>
       <c r="F37" s="52"/>
       <c r="G37" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H37" s="53">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I37" s="54" t="s">
         <v>20</v>
       </c>
       <c r="J37" s="55" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K37" s="56" t="s">
         <v>20</v>
       </c>
       <c r="L37" s="57" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M37" s="58"/>
-      <c r="N37" s="58" t="s">
-        <v>32</v>
-      </c>
+      <c r="N37" s="58"/>
       <c r="O37" s="52"/>
       <c r="P37" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q37" s="59">
-        <v>6</v>
-      </c>
-      <c r="R37" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="S37" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="T37" s="65" t="s">
-        <v>195</v>
-      </c>
-      <c r="U37" s="59" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q37" s="59"/>
+      <c r="R37" s="60"/>
+      <c r="S37" s="59"/>
+      <c r="T37" s="65"/>
+      <c r="U37" s="59"/>
+    </row>
+    <row r="38" spans="1:21" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
         <v>17</v>
       </c>
@@ -3708,7 +3689,7 @@
         <v>122</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D38" s="51" t="s">
         <v>192</v>
@@ -3716,16 +3697,16 @@
       <c r="E38" s="62"/>
       <c r="F38" s="52"/>
       <c r="G38" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H38" s="53">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I38" s="54" t="s">
-        <v>197</v>
+        <v>20</v>
       </c>
       <c r="J38" s="55" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K38" s="56" t="s">
         <v>20</v>
@@ -3735,11 +3716,11 @@
       </c>
       <c r="M38" s="58"/>
       <c r="N38" s="58" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="O38" s="52"/>
       <c r="P38" s="52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q38" s="59">
         <v>6</v>
@@ -3751,34 +3732,68 @@
         <v>127</v>
       </c>
       <c r="T38" s="65" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="U38" s="59" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="66"/>
-      <c r="U39" s="10"/>
+    <row r="39" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>251</v>
+      </c>
+      <c r="D39" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="E39" s="62"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="H39" s="53">
+        <v>33</v>
+      </c>
+      <c r="I39" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="J39" s="55" t="s">
+        <v>262</v>
+      </c>
+      <c r="K39" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="M39" s="58"/>
+      <c r="N39" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="O39" s="52"/>
+      <c r="P39" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q39" s="59">
+        <v>6</v>
+      </c>
+      <c r="R39" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="S39" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T39" s="65" t="s">
+        <v>198</v>
+      </c>
+      <c r="U39" s="59" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
@@ -4539,193 +4554,216 @@
       <c r="T72" s="66"/>
       <c r="U72" s="10"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>92</v>
-      </c>
+    <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="63"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="20"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="8"/>
+      <c r="O73" s="9"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="10"/>
+      <c r="R73" s="11"/>
+      <c r="S73" s="10"/>
+      <c r="T73" s="66"/>
+      <c r="U73" s="10"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U38"/>
+  <autoFilter ref="A2:U39"/>
   <mergeCells count="20">
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4757,31 +4795,31 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N72</xm:sqref>
+          <xm:sqref>N3:N73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A72</xm:sqref>
+          <xm:sqref>A3:A73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K72 P3:P72 I3:I72</xm:sqref>
+          <xm:sqref>K3:K73 P3:P73 I3:I73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L72</xm:sqref>
+          <xm:sqref>L3:L73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M72</xm:sqref>
+          <xm:sqref>M3:M73</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>